<commit_message>
Actualizada la plantilla de planificacion
</commit_message>
<xml_diff>
--- a/Plantilla_Planificacion/Plantilla_Planificacion_Proyecto.xlsx
+++ b/Plantilla_Planificacion/Plantilla_Planificacion_Proyecto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Industria 4.0\Desktop\Clase\uni1819\Segundo Semestre\Programacion II\Programas2\Plantilla_Planificacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4809A536-5A57-45A6-B7CC-CF4556DB2592}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA804CBF-9181-4F54-833F-E5E77F32CEE8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tareas" sheetId="1" r:id="rId1"/>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="103">
   <si>
     <t>Planificación del proyecto</t>
   </si>
@@ -387,6 +387,54 @@
   </si>
   <si>
     <t>Utilizacion de codigo externo que no conseguimos adecuar totalmente a nuestra aplicación.</t>
+  </si>
+  <si>
+    <t>Solucionar los parseos para las fechas</t>
+  </si>
+  <si>
+    <t>Encontramos codigo en StackOverFlow para solucionar los del parseo de fechas pero nos surgio otro problema.</t>
+  </si>
+  <si>
+    <t>Correcto formateo de las fechas</t>
+  </si>
+  <si>
+    <t>2 horas</t>
+  </si>
+  <si>
+    <t>Tratamos de implementar diferentes formatos para los tipos de aatributos Date pero sin éxito. Queremos lograr que la fecha nos la devuelva en formato nuumérico 00-00-0000 (dd-MM-yyyy) pero no lo logramos</t>
+  </si>
+  <si>
+    <t>Problemas con Git</t>
+  </si>
+  <si>
+    <t>Problemas al insertar el driver de conexión con BD</t>
+  </si>
+  <si>
+    <t>Dudas a cerca de las Propiedades relacionadas con el tipo de dato "DATE"</t>
+  </si>
+  <si>
+    <t>Estructuramiento de la parte LD</t>
+  </si>
+  <si>
+    <t>15 minutos</t>
+  </si>
+  <si>
+    <t>No supimos como insertar el driver para la conexión con la DB y nos supuso una desconfiguración del proyecto</t>
+  </si>
+  <si>
+    <t>Se nos desconfiguro el fichero .classpath y al subirlo a git nos dio problemas (no conseguimos subirlo ni actualizarlo). Lo solucionamo copiando el fichero .classpath del git y borrando el que teniamos en el proyecto.</t>
+  </si>
+  <si>
+    <t>No sabemos como aplicar propiedade al tipo de dato DATE (generar otro metodo o combertilo a String)</t>
+  </si>
+  <si>
+    <t>No tenemos una idea clara de como estructurar la parte de LD en el proyecto y tampoco como relacionar las propiedades para hacer las cosultas, inserts, deletes…</t>
+  </si>
+  <si>
+    <t>Dudas con los ArrayList</t>
+  </si>
+  <si>
+    <t>Donde hacer la llama de los ArrayList para guardar los objetos puesto que tenemos submenus y necesitamo regresar de unos a otros.</t>
   </si>
 </sst>
 </file>
@@ -1184,33 +1232,28 @@
     <xf numFmtId="16" fontId="2" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="2" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1233,31 +1276,36 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="2" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1540,7 +1588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1553,12 +1601,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -2867,8 +2915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S20" sqref="S20:S21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2886,10 +2934,10 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="59" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="16" t="s">
@@ -2912,13 +2960,13 @@
       <c r="P2" s="20"/>
       <c r="Q2" s="20"/>
       <c r="R2" s="22"/>
-      <c r="S2" s="68" t="s">
+      <c r="S2" s="61" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="77"/>
-      <c r="B3" s="67"/>
+      <c r="A3" s="71"/>
+      <c r="B3" s="60"/>
       <c r="C3" s="24" t="s">
         <v>42</v>
       </c>
@@ -2981,7 +3029,7 @@
         <f t="shared" si="0"/>
         <v>43605</v>
       </c>
-      <c r="S3" s="69"/>
+      <c r="S3" s="62"/>
     </row>
     <row r="4" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
@@ -3011,7 +3059,7 @@
       <c r="P4" s="32"/>
       <c r="Q4" s="32"/>
       <c r="R4" s="32"/>
-      <c r="S4" s="70" t="s">
+      <c r="S4" s="63" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3038,7 +3086,7 @@
       <c r="P5" s="38"/>
       <c r="Q5" s="38"/>
       <c r="R5" s="38"/>
-      <c r="S5" s="71"/>
+      <c r="S5" s="64"/>
     </row>
     <row r="6" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
@@ -3069,7 +3117,7 @@
       <c r="P6" s="32"/>
       <c r="Q6" s="32"/>
       <c r="R6" s="32"/>
-      <c r="S6" s="72" t="s">
+      <c r="S6" s="65" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3097,7 +3145,7 @@
       <c r="P7" s="38"/>
       <c r="Q7" s="38"/>
       <c r="R7" s="38"/>
-      <c r="S7" s="71"/>
+      <c r="S7" s="64"/>
     </row>
     <row r="8" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -3105,7 +3153,7 @@
       </c>
       <c r="B8" s="27">
         <f>SUM(D8:R8)</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.25</v>
       </c>
       <c r="C8" s="28" t="str">
         <f>IF(OR(SUM(D8:O8)=0,$A9=""),"",SUM(D8:O8))</f>
@@ -3118,7 +3166,9 @@
       <c r="H8" s="29">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="I8" s="32"/>
+      <c r="I8" s="29">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="J8" s="32"/>
       <c r="K8" s="32"/>
       <c r="L8" s="32"/>
@@ -3128,7 +3178,7 @@
       <c r="P8" s="32"/>
       <c r="Q8" s="32"/>
       <c r="R8" s="32"/>
-      <c r="S8" s="72" t="s">
+      <c r="S8" s="65" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3137,7 +3187,7 @@
       <c r="B9" s="35"/>
       <c r="C9" s="28">
         <f>SUM(D9:S9)</f>
-        <v>0.125</v>
+        <v>0.52083333333333326</v>
       </c>
       <c r="D9" s="38"/>
       <c r="E9" s="38"/>
@@ -3146,7 +3196,9 @@
       <c r="H9" s="37">
         <v>0.125</v>
       </c>
-      <c r="I9" s="38"/>
+      <c r="I9" s="37">
+        <v>0.39583333333333331</v>
+      </c>
       <c r="J9" s="38"/>
       <c r="K9" s="38"/>
       <c r="L9" s="38"/>
@@ -3156,7 +3208,7 @@
       <c r="P9" s="38"/>
       <c r="Q9" s="38"/>
       <c r="R9" s="38"/>
-      <c r="S9" s="79"/>
+      <c r="S9" s="72"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
@@ -3185,7 +3237,7 @@
       <c r="P10" s="32"/>
       <c r="Q10" s="32"/>
       <c r="R10" s="32"/>
-      <c r="S10" s="72"/>
+      <c r="S10" s="65"/>
     </row>
     <row r="11" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="40"/>
@@ -3209,7 +3261,7 @@
       <c r="P11" s="38"/>
       <c r="Q11" s="38"/>
       <c r="R11" s="38"/>
-      <c r="S11" s="79"/>
+      <c r="S11" s="72"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
@@ -3238,7 +3290,7 @@
       <c r="P12" s="32"/>
       <c r="Q12" s="32"/>
       <c r="R12" s="32"/>
-      <c r="S12" s="72"/>
+      <c r="S12" s="65"/>
     </row>
     <row r="13" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="40"/>
@@ -3262,7 +3314,7 @@
       <c r="P13" s="38"/>
       <c r="Q13" s="38"/>
       <c r="R13" s="38"/>
-      <c r="S13" s="79"/>
+      <c r="S13" s="72"/>
     </row>
     <row r="14" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
@@ -3291,7 +3343,7 @@
       <c r="P14" s="32"/>
       <c r="Q14" s="32"/>
       <c r="R14" s="32"/>
-      <c r="S14" s="72"/>
+      <c r="S14" s="65"/>
     </row>
     <row r="15" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="40"/>
@@ -3315,7 +3367,7 @@
       <c r="P15" s="38"/>
       <c r="Q15" s="38"/>
       <c r="R15" s="38"/>
-      <c r="S15" s="79"/>
+      <c r="S15" s="72"/>
     </row>
     <row r="16" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
@@ -3344,7 +3396,7 @@
       <c r="P16" s="32"/>
       <c r="Q16" s="32"/>
       <c r="R16" s="32"/>
-      <c r="S16" s="72"/>
+      <c r="S16" s="65"/>
     </row>
     <row r="17" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="40"/>
@@ -3368,7 +3420,7 @@
       <c r="P17" s="38"/>
       <c r="Q17" s="38"/>
       <c r="R17" s="38"/>
-      <c r="S17" s="79"/>
+      <c r="S17" s="72"/>
     </row>
     <row r="18" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
@@ -3394,7 +3446,7 @@
       <c r="P18" s="32"/>
       <c r="Q18" s="32"/>
       <c r="R18" s="32"/>
-      <c r="S18" s="72"/>
+      <c r="S18" s="65"/>
     </row>
     <row r="19" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="40"/>
@@ -3421,7 +3473,7 @@
       <c r="P19" s="38"/>
       <c r="Q19" s="38"/>
       <c r="R19" s="38"/>
-      <c r="S19" s="79"/>
+      <c r="S19" s="72"/>
     </row>
     <row r="20" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
@@ -3450,7 +3502,7 @@
       <c r="P20" s="32"/>
       <c r="Q20" s="32"/>
       <c r="R20" s="32"/>
-      <c r="S20" s="72"/>
+      <c r="S20" s="65"/>
     </row>
     <row r="21" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
@@ -3477,19 +3529,19 @@
       <c r="P21" s="38"/>
       <c r="Q21" s="38"/>
       <c r="R21" s="38"/>
-      <c r="S21" s="79"/>
+      <c r="S21" s="72"/>
     </row>
     <row r="22" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="73" t="s">
+      <c r="A22" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="75">
+      <c r="B22" s="68">
         <f>SUM(B4:B21)</f>
-        <v>4.145833333333333</v>
-      </c>
-      <c r="C22" s="58">
+        <v>4.3125</v>
+      </c>
+      <c r="C22" s="78">
         <f>SUM(C5:C21)</f>
-        <v>0.35416666666666669</v>
+        <v>0.75</v>
       </c>
       <c r="D22" s="42">
         <f t="shared" ref="D22:R22" si="1">SUM(D4,D6,D8,D10,D12,D14,D16,D18,D20)</f>
@@ -3513,7 +3565,7 @@
       </c>
       <c r="I22" s="43">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="J22" s="43">
         <f t="shared" si="1"/>
@@ -3551,12 +3603,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S22" s="80"/>
+      <c r="S22" s="52"/>
     </row>
     <row r="23" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="74"/>
-      <c r="B23" s="59"/>
-      <c r="C23" s="59"/>
+      <c r="A23" s="67"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="69"/>
       <c r="D23" s="44">
         <f t="shared" ref="D23:R23" si="2">SUM(D5,D7,D9,D11,D13,D15,D17,D19,D21)</f>
         <v>0.125</v>
@@ -3579,7 +3631,7 @@
       </c>
       <c r="I23" s="45">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="J23" s="45">
         <f t="shared" si="2"/>
@@ -3677,13 +3729,13 @@
       <c r="S26" s="46"/>
     </row>
     <row r="27" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="60" t="s">
+      <c r="B27" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="61"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="62"/>
+      <c r="C27" s="80"/>
+      <c r="D27" s="80"/>
+      <c r="E27" s="80"/>
+      <c r="F27" s="81"/>
       <c r="G27" s="46"/>
       <c r="H27" s="46"/>
       <c r="I27" s="46"/>
@@ -3702,58 +3754,58 @@
       <c r="B28" s="47">
         <v>43513</v>
       </c>
-      <c r="C28" s="63" t="s">
+      <c r="C28" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="65"/>
+      <c r="D28" s="83"/>
+      <c r="E28" s="83"/>
+      <c r="F28" s="84"/>
     </row>
     <row r="29" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="48"/>
-      <c r="C29" s="56" t="s">
+      <c r="C29" s="76" t="s">
         <v>69</v>
       </c>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="57"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="77"/>
     </row>
     <row r="30" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="48"/>
-      <c r="C30" s="56" t="s">
+      <c r="C30" s="76" t="s">
         <v>70</v>
       </c>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="57"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="77"/>
     </row>
     <row r="31" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="48"/>
-      <c r="C31" s="56" t="s">
+      <c r="C31" s="76" t="s">
         <v>71</v>
       </c>
-      <c r="D31" s="52"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="57"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="77"/>
     </row>
     <row r="32" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="48"/>
-      <c r="C32" s="56" t="s">
+      <c r="C32" s="76" t="s">
         <v>72</v>
       </c>
-      <c r="D32" s="52"/>
-      <c r="E32" s="52"/>
-      <c r="F32" s="57"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="77"/>
     </row>
     <row r="33" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="49"/>
       <c r="B33" s="50"/>
-      <c r="C33" s="53" t="s">
+      <c r="C33" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="D33" s="54"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="55"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="75"/>
     </row>
     <row r="34" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4724,6 +4776,14 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C31:F31"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="S4:S5"/>
@@ -4738,14 +4798,6 @@
     <mergeCell ref="S16:S17"/>
     <mergeCell ref="S18:S19"/>
     <mergeCell ref="S20:S21"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -4756,8 +4808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4826,195 +4878,265 @@
       <c r="A4" s="3">
         <v>43537</v>
       </c>
-      <c r="B4" s="81" t="s">
+      <c r="B4" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="81" t="s">
+      <c r="C4" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="D4" s="82" t="s">
+      <c r="D4" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="81" t="s">
+      <c r="E4" s="53" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="83">
+      <c r="A5" s="55">
         <v>43537</v>
       </c>
-      <c r="B5" s="78" t="s">
+      <c r="B5" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="81" t="s">
+      <c r="C5" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="82" t="s">
+      <c r="D5" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="81" t="s">
+      <c r="E5" s="53" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="83">
+      <c r="A6" s="55">
         <v>43537</v>
       </c>
-      <c r="B6" s="78" t="s">
+      <c r="B6" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="81" t="s">
+      <c r="C6" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="82" t="s">
+      <c r="D6" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="E6" s="81" t="s">
+      <c r="E6" s="53" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="83">
+      <c r="A7" s="55">
         <v>43538</v>
       </c>
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="81" t="s">
+      <c r="C7" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="82" t="s">
+      <c r="D7" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="E7" s="81" t="s">
+      <c r="E7" s="53" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="83"/>
-      <c r="B8" s="78"/>
-      <c r="C8" s="78"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="78"/>
-    </row>
-    <row r="9" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="83"/>
-      <c r="B9" s="78"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="78"/>
-    </row>
-    <row r="10" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="83"/>
-      <c r="B10" s="78"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="78"/>
-    </row>
-    <row r="11" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="83"/>
-      <c r="B11" s="78"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="78"/>
-    </row>
-    <row r="12" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="83"/>
-      <c r="B12" s="78"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="78"/>
-    </row>
-    <row r="13" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="83"/>
-      <c r="B13" s="78"/>
-      <c r="C13" s="78"/>
-      <c r="D13" s="84"/>
-      <c r="E13" s="78"/>
-    </row>
-    <row r="14" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="83"/>
-      <c r="B14" s="78"/>
-      <c r="C14" s="78"/>
-      <c r="D14" s="84"/>
-      <c r="E14" s="78"/>
+    <row r="8" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="55">
+        <v>43542</v>
+      </c>
+      <c r="B8" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="51" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="55">
+        <v>43542</v>
+      </c>
+      <c r="B9" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="51" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="55">
+        <v>43543</v>
+      </c>
+      <c r="B10" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="51" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="55">
+        <v>43543</v>
+      </c>
+      <c r="B11" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="51" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="51" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="55">
+        <v>43543</v>
+      </c>
+      <c r="B12" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" s="51" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="55">
+        <v>43544</v>
+      </c>
+      <c r="B13" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="51" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="55">
+        <v>43544</v>
+      </c>
+      <c r="B14" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="51" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="51" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="83"/>
-      <c r="B15" s="78"/>
-      <c r="C15" s="78"/>
-      <c r="D15" s="84"/>
-      <c r="E15" s="78"/>
+      <c r="A15" s="55"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="51"/>
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="83"/>
-      <c r="B16" s="78"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="84"/>
-      <c r="E16" s="78"/>
+      <c r="A16" s="55"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="51"/>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="83"/>
-      <c r="B17" s="78"/>
-      <c r="C17" s="78"/>
-      <c r="D17" s="84"/>
-      <c r="E17" s="78"/>
+      <c r="A17" s="55"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="51"/>
     </row>
     <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="83"/>
-      <c r="B18" s="78"/>
-      <c r="C18" s="78"/>
-      <c r="D18" s="84"/>
-      <c r="E18" s="78"/>
+      <c r="A18" s="55"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="51"/>
     </row>
     <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="83"/>
-      <c r="B19" s="78"/>
-      <c r="C19" s="78"/>
-      <c r="D19" s="84"/>
-      <c r="E19" s="78"/>
+      <c r="A19" s="55"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="51"/>
     </row>
     <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="83"/>
-      <c r="B20" s="78"/>
-      <c r="C20" s="78"/>
-      <c r="D20" s="84"/>
-      <c r="E20" s="78"/>
+      <c r="A20" s="55"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="51"/>
     </row>
     <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="83"/>
-      <c r="B21" s="78"/>
-      <c r="C21" s="78"/>
-      <c r="D21" s="84"/>
-      <c r="E21" s="78"/>
+      <c r="A21" s="55"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="51"/>
     </row>
     <row r="22" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="83"/>
-      <c r="B22" s="78"/>
-      <c r="C22" s="78"/>
-      <c r="D22" s="84"/>
-      <c r="E22" s="78"/>
+      <c r="A22" s="55"/>
+      <c r="B22" s="51"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="51"/>
     </row>
     <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="83"/>
-      <c r="B23" s="78"/>
-      <c r="C23" s="78"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="78"/>
+      <c r="A23" s="55"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="51"/>
     </row>
     <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="83"/>
-      <c r="B24" s="78"/>
-      <c r="C24" s="78"/>
-      <c r="D24" s="84"/>
-      <c r="E24" s="78"/>
+      <c r="A24" s="55"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="51"/>
     </row>
     <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="83"/>
-      <c r="B25" s="78"/>
-      <c r="C25" s="78"/>
-      <c r="D25" s="84"/>
-      <c r="E25" s="78"/>
+      <c r="A25" s="55"/>
+      <c r="B25" s="51"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="51"/>
     </row>
     <row r="26" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>

</xml_diff>

<commit_message>
actualizada la plantilla 23/03/19
</commit_message>
<xml_diff>
--- a/Plantilla_Planificacion/Plantilla_Planificacion_Proyecto.xlsx
+++ b/Plantilla_Planificacion/Plantilla_Planificacion_Proyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Industria 4.0\Desktop\Clase\uni1819\Segundo Semestre\Programacion II\Programas2\Plantilla_Planificacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA804CBF-9181-4F54-833F-E5E77F32CEE8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A46797-741A-4B22-8011-B29B71371CC2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="105">
   <si>
     <t>Planificación del proyecto</t>
   </si>
@@ -435,6 +435,12 @@
   </si>
   <si>
     <t>Donde hacer la llama de los ArrayList para guardar los objetos puesto que tenemos submenus y necesitamo regresar de unos a otros.</t>
+  </si>
+  <si>
+    <t>Problemas con el ArrayList de sacar datos de BD</t>
+  </si>
+  <si>
+    <t>Al sacar los datos de BD, hacer los objetos y meterlos en ArrayList nos duplicaba la informacion según haciamos consultas.</t>
   </si>
 </sst>
 </file>
@@ -1110,7 +1116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1254,6 +1260,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="2" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1276,7 +1305,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1284,28 +1312,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="2" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2916,7 +2925,7 @@
   <dimension ref="A1:S1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2934,10 +2943,10 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="72" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="16" t="s">
@@ -2960,13 +2969,13 @@
       <c r="P2" s="20"/>
       <c r="Q2" s="20"/>
       <c r="R2" s="22"/>
-      <c r="S2" s="61" t="s">
+      <c r="S2" s="74" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="71"/>
-      <c r="B3" s="60"/>
+      <c r="A3" s="83"/>
+      <c r="B3" s="73"/>
       <c r="C3" s="24" t="s">
         <v>42</v>
       </c>
@@ -3029,7 +3038,7 @@
         <f t="shared" si="0"/>
         <v>43605</v>
       </c>
-      <c r="S3" s="62"/>
+      <c r="S3" s="75"/>
     </row>
     <row r="4" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
@@ -3059,7 +3068,7 @@
       <c r="P4" s="32"/>
       <c r="Q4" s="32"/>
       <c r="R4" s="32"/>
-      <c r="S4" s="63" t="s">
+      <c r="S4" s="76" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3086,7 +3095,7 @@
       <c r="P5" s="38"/>
       <c r="Q5" s="38"/>
       <c r="R5" s="38"/>
-      <c r="S5" s="64"/>
+      <c r="S5" s="77"/>
     </row>
     <row r="6" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
@@ -3117,7 +3126,7 @@
       <c r="P6" s="32"/>
       <c r="Q6" s="32"/>
       <c r="R6" s="32"/>
-      <c r="S6" s="65" t="s">
+      <c r="S6" s="78" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3145,7 +3154,7 @@
       <c r="P7" s="38"/>
       <c r="Q7" s="38"/>
       <c r="R7" s="38"/>
-      <c r="S7" s="64"/>
+      <c r="S7" s="77"/>
     </row>
     <row r="8" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -3173,12 +3182,12 @@
       <c r="K8" s="32"/>
       <c r="L8" s="32"/>
       <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
+      <c r="N8" s="85"/>
       <c r="O8" s="32"/>
       <c r="P8" s="32"/>
       <c r="Q8" s="32"/>
       <c r="R8" s="32"/>
-      <c r="S8" s="65" t="s">
+      <c r="S8" s="78" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3187,7 +3196,7 @@
       <c r="B9" s="35"/>
       <c r="C9" s="28">
         <f>SUM(D9:S9)</f>
-        <v>0.52083333333333326</v>
+        <v>0.53125</v>
       </c>
       <c r="D9" s="38"/>
       <c r="E9" s="38"/>
@@ -3197,7 +3206,7 @@
         <v>0.125</v>
       </c>
       <c r="I9" s="37">
-        <v>0.39583333333333331</v>
+        <v>0.40625</v>
       </c>
       <c r="J9" s="38"/>
       <c r="K9" s="38"/>
@@ -3208,7 +3217,7 @@
       <c r="P9" s="38"/>
       <c r="Q9" s="38"/>
       <c r="R9" s="38"/>
-      <c r="S9" s="72"/>
+      <c r="S9" s="84"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
@@ -3237,7 +3246,7 @@
       <c r="P10" s="32"/>
       <c r="Q10" s="32"/>
       <c r="R10" s="32"/>
-      <c r="S10" s="65"/>
+      <c r="S10" s="78"/>
     </row>
     <row r="11" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="40"/>
@@ -3261,7 +3270,7 @@
       <c r="P11" s="38"/>
       <c r="Q11" s="38"/>
       <c r="R11" s="38"/>
-      <c r="S11" s="72"/>
+      <c r="S11" s="84"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
@@ -3290,7 +3299,7 @@
       <c r="P12" s="32"/>
       <c r="Q12" s="32"/>
       <c r="R12" s="32"/>
-      <c r="S12" s="65"/>
+      <c r="S12" s="78"/>
     </row>
     <row r="13" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="40"/>
@@ -3314,7 +3323,7 @@
       <c r="P13" s="38"/>
       <c r="Q13" s="38"/>
       <c r="R13" s="38"/>
-      <c r="S13" s="72"/>
+      <c r="S13" s="84"/>
     </row>
     <row r="14" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
@@ -3343,7 +3352,7 @@
       <c r="P14" s="32"/>
       <c r="Q14" s="32"/>
       <c r="R14" s="32"/>
-      <c r="S14" s="65"/>
+      <c r="S14" s="78"/>
     </row>
     <row r="15" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="40"/>
@@ -3367,7 +3376,7 @@
       <c r="P15" s="38"/>
       <c r="Q15" s="38"/>
       <c r="R15" s="38"/>
-      <c r="S15" s="72"/>
+      <c r="S15" s="84"/>
     </row>
     <row r="16" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
@@ -3396,7 +3405,7 @@
       <c r="P16" s="32"/>
       <c r="Q16" s="32"/>
       <c r="R16" s="32"/>
-      <c r="S16" s="65"/>
+      <c r="S16" s="78"/>
     </row>
     <row r="17" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="40"/>
@@ -3420,7 +3429,7 @@
       <c r="P17" s="38"/>
       <c r="Q17" s="38"/>
       <c r="R17" s="38"/>
-      <c r="S17" s="72"/>
+      <c r="S17" s="84"/>
     </row>
     <row r="18" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
@@ -3446,7 +3455,7 @@
       <c r="P18" s="32"/>
       <c r="Q18" s="32"/>
       <c r="R18" s="32"/>
-      <c r="S18" s="65"/>
+      <c r="S18" s="78"/>
     </row>
     <row r="19" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="40"/>
@@ -3473,7 +3482,7 @@
       <c r="P19" s="38"/>
       <c r="Q19" s="38"/>
       <c r="R19" s="38"/>
-      <c r="S19" s="72"/>
+      <c r="S19" s="84"/>
     </row>
     <row r="20" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
@@ -3502,7 +3511,7 @@
       <c r="P20" s="32"/>
       <c r="Q20" s="32"/>
       <c r="R20" s="32"/>
-      <c r="S20" s="65"/>
+      <c r="S20" s="78"/>
     </row>
     <row r="21" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
@@ -3529,19 +3538,19 @@
       <c r="P21" s="38"/>
       <c r="Q21" s="38"/>
       <c r="R21" s="38"/>
-      <c r="S21" s="72"/>
+      <c r="S21" s="84"/>
     </row>
     <row r="22" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="79" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="68">
+      <c r="B22" s="81">
         <f>SUM(B4:B21)</f>
         <v>4.3125</v>
       </c>
-      <c r="C22" s="78">
+      <c r="C22" s="64">
         <f>SUM(C5:C21)</f>
-        <v>0.75</v>
+        <v>0.76041666666666674</v>
       </c>
       <c r="D22" s="42">
         <f t="shared" ref="D22:R22" si="1">SUM(D4,D6,D8,D10,D12,D14,D16,D18,D20)</f>
@@ -3606,9 +3615,9 @@
       <c r="S22" s="52"/>
     </row>
     <row r="23" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="67"/>
-      <c r="B23" s="69"/>
-      <c r="C23" s="69"/>
+      <c r="A23" s="80"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="65"/>
       <c r="D23" s="44">
         <f t="shared" ref="D23:R23" si="2">SUM(D5,D7,D9,D11,D13,D15,D17,D19,D21)</f>
         <v>0.125</v>
@@ -3631,7 +3640,7 @@
       </c>
       <c r="I23" s="45">
         <f t="shared" si="2"/>
-        <v>0.39583333333333331</v>
+        <v>0.40625</v>
       </c>
       <c r="J23" s="45">
         <f t="shared" si="2"/>
@@ -3729,13 +3738,13 @@
       <c r="S26" s="46"/>
     </row>
     <row r="27" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="79" t="s">
+      <c r="B27" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="80"/>
-      <c r="D27" s="80"/>
-      <c r="E27" s="80"/>
-      <c r="F27" s="81"/>
+      <c r="C27" s="67"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="68"/>
       <c r="G27" s="46"/>
       <c r="H27" s="46"/>
       <c r="I27" s="46"/>
@@ -3754,58 +3763,58 @@
       <c r="B28" s="47">
         <v>43513</v>
       </c>
-      <c r="C28" s="82" t="s">
+      <c r="C28" s="69" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="83"/>
-      <c r="E28" s="83"/>
-      <c r="F28" s="84"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="71"/>
     </row>
     <row r="29" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="48"/>
-      <c r="C29" s="76" t="s">
+      <c r="C29" s="62" t="s">
         <v>69</v>
       </c>
       <c r="D29" s="58"/>
       <c r="E29" s="58"/>
-      <c r="F29" s="77"/>
+      <c r="F29" s="63"/>
     </row>
     <row r="30" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="48"/>
-      <c r="C30" s="76" t="s">
+      <c r="C30" s="62" t="s">
         <v>70</v>
       </c>
       <c r="D30" s="58"/>
       <c r="E30" s="58"/>
-      <c r="F30" s="77"/>
+      <c r="F30" s="63"/>
     </row>
     <row r="31" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="48"/>
-      <c r="C31" s="76" t="s">
+      <c r="C31" s="62" t="s">
         <v>71</v>
       </c>
       <c r="D31" s="58"/>
       <c r="E31" s="58"/>
-      <c r="F31" s="77"/>
+      <c r="F31" s="63"/>
     </row>
     <row r="32" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="48"/>
-      <c r="C32" s="76" t="s">
+      <c r="C32" s="62" t="s">
         <v>72</v>
       </c>
       <c r="D32" s="58"/>
       <c r="E32" s="58"/>
-      <c r="F32" s="77"/>
+      <c r="F32" s="63"/>
     </row>
     <row r="33" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="49"/>
       <c r="B33" s="50"/>
-      <c r="C33" s="73" t="s">
+      <c r="C33" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="D33" s="74"/>
-      <c r="E33" s="74"/>
-      <c r="F33" s="75"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="61"/>
     </row>
     <row r="34" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4776,14 +4785,6 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C31:F31"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="S4:S5"/>
@@ -4798,9 +4799,17 @@
     <mergeCell ref="S16:S17"/>
     <mergeCell ref="S18:S19"/>
     <mergeCell ref="S20:S21"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4808,8 +4817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5061,12 +5070,22 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="55"/>
-      <c r="B15" s="51"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="51"/>
+    <row r="15" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="55">
+        <v>43545</v>
+      </c>
+      <c r="B15" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="51" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" s="51" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="55"/>

</xml_diff>

<commit_message>
actualizada plantilla hasta la entrega de tarea_02
</commit_message>
<xml_diff>
--- a/Plantilla_Planificacion/Plantilla_Planificacion_Proyecto.xlsx
+++ b/Plantilla_Planificacion/Plantilla_Planificacion_Proyecto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Industria 4.0\Desktop\Clase\uni1819\Segundo Semestre\Programacion II\Programas2\Plantilla_Planificacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A46797-741A-4B22-8011-B29B71371CC2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728C4E52-CDA9-4F1B-A7A4-1189D9F9CE05}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tareas" sheetId="1" r:id="rId1"/>
@@ -1256,33 +1256,13 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="2" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1305,6 +1285,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1312,9 +1293,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="2" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1597,7 +1597,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1610,12 +1612,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
     </row>
     <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -1702,8 +1704,12 @@
       <c r="C8" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="19"/>
+      <c r="D8" s="21">
+        <v>0.25</v>
+      </c>
+      <c r="E8" s="23">
+        <v>0.53125</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -2924,8 +2930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2943,10 +2949,10 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="60" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="16" t="s">
@@ -2969,13 +2975,13 @@
       <c r="P2" s="20"/>
       <c r="Q2" s="20"/>
       <c r="R2" s="22"/>
-      <c r="S2" s="74" t="s">
+      <c r="S2" s="62" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="83"/>
-      <c r="B3" s="73"/>
+      <c r="A3" s="72"/>
+      <c r="B3" s="61"/>
       <c r="C3" s="24" t="s">
         <v>42</v>
       </c>
@@ -3038,7 +3044,7 @@
         <f t="shared" si="0"/>
         <v>43605</v>
       </c>
-      <c r="S3" s="75"/>
+      <c r="S3" s="63"/>
     </row>
     <row r="4" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
@@ -3068,7 +3074,7 @@
       <c r="P4" s="32"/>
       <c r="Q4" s="32"/>
       <c r="R4" s="32"/>
-      <c r="S4" s="76" t="s">
+      <c r="S4" s="64" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3095,7 +3101,7 @@
       <c r="P5" s="38"/>
       <c r="Q5" s="38"/>
       <c r="R5" s="38"/>
-      <c r="S5" s="77"/>
+      <c r="S5" s="65"/>
     </row>
     <row r="6" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
@@ -3126,7 +3132,7 @@
       <c r="P6" s="32"/>
       <c r="Q6" s="32"/>
       <c r="R6" s="32"/>
-      <c r="S6" s="78" t="s">
+      <c r="S6" s="66" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3154,7 +3160,7 @@
       <c r="P7" s="38"/>
       <c r="Q7" s="38"/>
       <c r="R7" s="38"/>
-      <c r="S7" s="77"/>
+      <c r="S7" s="65"/>
     </row>
     <row r="8" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -3182,12 +3188,12 @@
       <c r="K8" s="32"/>
       <c r="L8" s="32"/>
       <c r="M8" s="32"/>
-      <c r="N8" s="85"/>
+      <c r="N8" s="57"/>
       <c r="O8" s="32"/>
       <c r="P8" s="32"/>
       <c r="Q8" s="32"/>
       <c r="R8" s="32"/>
-      <c r="S8" s="78" t="s">
+      <c r="S8" s="66" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3217,7 +3223,7 @@
       <c r="P9" s="38"/>
       <c r="Q9" s="38"/>
       <c r="R9" s="38"/>
-      <c r="S9" s="84"/>
+      <c r="S9" s="73"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
@@ -3246,7 +3252,7 @@
       <c r="P10" s="32"/>
       <c r="Q10" s="32"/>
       <c r="R10" s="32"/>
-      <c r="S10" s="78"/>
+      <c r="S10" s="66"/>
     </row>
     <row r="11" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="40"/>
@@ -3270,7 +3276,7 @@
       <c r="P11" s="38"/>
       <c r="Q11" s="38"/>
       <c r="R11" s="38"/>
-      <c r="S11" s="84"/>
+      <c r="S11" s="73"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
@@ -3299,7 +3305,7 @@
       <c r="P12" s="32"/>
       <c r="Q12" s="32"/>
       <c r="R12" s="32"/>
-      <c r="S12" s="78"/>
+      <c r="S12" s="66"/>
     </row>
     <row r="13" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="40"/>
@@ -3323,7 +3329,7 @@
       <c r="P13" s="38"/>
       <c r="Q13" s="38"/>
       <c r="R13" s="38"/>
-      <c r="S13" s="84"/>
+      <c r="S13" s="73"/>
     </row>
     <row r="14" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
@@ -3352,7 +3358,7 @@
       <c r="P14" s="32"/>
       <c r="Q14" s="32"/>
       <c r="R14" s="32"/>
-      <c r="S14" s="78"/>
+      <c r="S14" s="66"/>
     </row>
     <row r="15" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="40"/>
@@ -3376,7 +3382,7 @@
       <c r="P15" s="38"/>
       <c r="Q15" s="38"/>
       <c r="R15" s="38"/>
-      <c r="S15" s="84"/>
+      <c r="S15" s="73"/>
     </row>
     <row r="16" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
@@ -3405,7 +3411,7 @@
       <c r="P16" s="32"/>
       <c r="Q16" s="32"/>
       <c r="R16" s="32"/>
-      <c r="S16" s="78"/>
+      <c r="S16" s="66"/>
     </row>
     <row r="17" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="40"/>
@@ -3429,7 +3435,7 @@
       <c r="P17" s="38"/>
       <c r="Q17" s="38"/>
       <c r="R17" s="38"/>
-      <c r="S17" s="84"/>
+      <c r="S17" s="73"/>
     </row>
     <row r="18" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
@@ -3455,7 +3461,7 @@
       <c r="P18" s="32"/>
       <c r="Q18" s="32"/>
       <c r="R18" s="32"/>
-      <c r="S18" s="78"/>
+      <c r="S18" s="66"/>
     </row>
     <row r="19" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="40"/>
@@ -3482,7 +3488,7 @@
       <c r="P19" s="38"/>
       <c r="Q19" s="38"/>
       <c r="R19" s="38"/>
-      <c r="S19" s="84"/>
+      <c r="S19" s="73"/>
     </row>
     <row r="20" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
@@ -3511,7 +3517,7 @@
       <c r="P20" s="32"/>
       <c r="Q20" s="32"/>
       <c r="R20" s="32"/>
-      <c r="S20" s="78"/>
+      <c r="S20" s="66"/>
     </row>
     <row r="21" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
@@ -3538,17 +3544,17 @@
       <c r="P21" s="38"/>
       <c r="Q21" s="38"/>
       <c r="R21" s="38"/>
-      <c r="S21" s="84"/>
+      <c r="S21" s="73"/>
     </row>
     <row r="22" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="79" t="s">
+      <c r="A22" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="81">
+      <c r="B22" s="69">
         <f>SUM(B4:B21)</f>
         <v>4.3125</v>
       </c>
-      <c r="C22" s="64">
+      <c r="C22" s="79">
         <f>SUM(C5:C21)</f>
         <v>0.76041666666666674</v>
       </c>
@@ -3615,9 +3621,9 @@
       <c r="S22" s="52"/>
     </row>
     <row r="23" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="80"/>
-      <c r="B23" s="65"/>
-      <c r="C23" s="65"/>
+      <c r="A23" s="68"/>
+      <c r="B23" s="70"/>
+      <c r="C23" s="70"/>
       <c r="D23" s="44">
         <f t="shared" ref="D23:R23" si="2">SUM(D5,D7,D9,D11,D13,D15,D17,D19,D21)</f>
         <v>0.125</v>
@@ -3738,13 +3744,13 @@
       <c r="S26" s="46"/>
     </row>
     <row r="27" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="66" t="s">
+      <c r="B27" s="80" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="67"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="67"/>
-      <c r="F27" s="68"/>
+      <c r="C27" s="81"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="82"/>
       <c r="G27" s="46"/>
       <c r="H27" s="46"/>
       <c r="I27" s="46"/>
@@ -3763,58 +3769,58 @@
       <c r="B28" s="47">
         <v>43513</v>
       </c>
-      <c r="C28" s="69" t="s">
+      <c r="C28" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="70"/>
-      <c r="E28" s="70"/>
-      <c r="F28" s="71"/>
+      <c r="D28" s="84"/>
+      <c r="E28" s="84"/>
+      <c r="F28" s="85"/>
     </row>
     <row r="29" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="48"/>
-      <c r="C29" s="62" t="s">
+      <c r="C29" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="D29" s="58"/>
-      <c r="E29" s="58"/>
-      <c r="F29" s="63"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="59"/>
+      <c r="F29" s="78"/>
     </row>
     <row r="30" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="48"/>
-      <c r="C30" s="62" t="s">
+      <c r="C30" s="77" t="s">
         <v>70</v>
       </c>
-      <c r="D30" s="58"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="63"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="78"/>
     </row>
     <row r="31" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="48"/>
-      <c r="C31" s="62" t="s">
+      <c r="C31" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="D31" s="58"/>
-      <c r="E31" s="58"/>
-      <c r="F31" s="63"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="59"/>
+      <c r="F31" s="78"/>
     </row>
     <row r="32" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="48"/>
-      <c r="C32" s="62" t="s">
+      <c r="C32" s="77" t="s">
         <v>72</v>
       </c>
-      <c r="D32" s="58"/>
-      <c r="E32" s="58"/>
-      <c r="F32" s="63"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="78"/>
     </row>
     <row r="33" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="49"/>
       <c r="B33" s="50"/>
-      <c r="C33" s="59" t="s">
+      <c r="C33" s="74" t="s">
         <v>73</v>
       </c>
-      <c r="D33" s="60"/>
-      <c r="E33" s="60"/>
-      <c r="F33" s="61"/>
+      <c r="D33" s="75"/>
+      <c r="E33" s="75"/>
+      <c r="F33" s="76"/>
     </row>
     <row r="34" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4785,6 +4791,14 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C31:F31"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="S4:S5"/>
@@ -4799,14 +4813,6 @@
     <mergeCell ref="S16:S17"/>
     <mergeCell ref="S18:S19"/>
     <mergeCell ref="S20:S21"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -4818,7 +4824,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
actualizacion de la plantilla
</commit_message>
<xml_diff>
--- a/Plantilla_Planificacion/Plantilla_Planificacion_Proyecto.xlsx
+++ b/Plantilla_Planificacion/Plantilla_Planificacion_Proyecto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Industria 4.0\Desktop\Clase\uni1819\Segundo Semestre\Programacion II\Programas2\Plantilla_Planificacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728C4E52-CDA9-4F1B-A7A4-1189D9F9CE05}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B17FF22-6977-4C2E-8D9B-C580EE031E4B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tareas" sheetId="1" r:id="rId1"/>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="114">
   <si>
     <t>Planificación del proyecto</t>
   </si>
@@ -441,6 +441,33 @@
   </si>
   <si>
     <t>Al sacar los datos de BD, hacer los objetos y meterlos en ArrayList nos duplicaba la informacion según haciamos consultas.</t>
+  </si>
+  <si>
+    <t>T03 Diseño de excepciones y gestión de errores en la aplicación y ordenación</t>
+  </si>
+  <si>
+    <t>Problemas con la BD</t>
+  </si>
+  <si>
+    <t>Al hacer la carga de datos de la BD a la aplicaccion no nos extraia la primera linea de datos.</t>
+  </si>
+  <si>
+    <t>Problemas con fechas</t>
+  </si>
+  <si>
+    <t>Problemas con un retorno de tipo boolean</t>
+  </si>
+  <si>
+    <t>Al recoger un dato boolean de BD nos sacaba un NULL por pantalla</t>
+  </si>
+  <si>
+    <t>Problemas con el borrado de Pedidos</t>
+  </si>
+  <si>
+    <t>Al intentar borrar de la tabla de pedidos nos fa errores</t>
+  </si>
+  <si>
+    <t>Tenemos problemas al insertar las fechas. Nos cambia el valor de las fechas</t>
   </si>
 </sst>
 </file>
@@ -1263,6 +1290,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="2" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1285,7 +1335,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1293,28 +1342,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="2" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1597,8 +1624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2931,7 +2958,7 @@
   <dimension ref="A1:S1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2949,10 +2976,10 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="73" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="16" t="s">
@@ -2975,13 +3002,13 @@
       <c r="P2" s="20"/>
       <c r="Q2" s="20"/>
       <c r="R2" s="22"/>
-      <c r="S2" s="62" t="s">
+      <c r="S2" s="75" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="72"/>
-      <c r="B3" s="61"/>
+      <c r="A3" s="84"/>
+      <c r="B3" s="74"/>
       <c r="C3" s="24" t="s">
         <v>42</v>
       </c>
@@ -3044,7 +3071,7 @@
         <f t="shared" si="0"/>
         <v>43605</v>
       </c>
-      <c r="S3" s="63"/>
+      <c r="S3" s="76"/>
     </row>
     <row r="4" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
@@ -3074,7 +3101,7 @@
       <c r="P4" s="32"/>
       <c r="Q4" s="32"/>
       <c r="R4" s="32"/>
-      <c r="S4" s="64" t="s">
+      <c r="S4" s="77" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3101,7 +3128,7 @@
       <c r="P5" s="38"/>
       <c r="Q5" s="38"/>
       <c r="R5" s="38"/>
-      <c r="S5" s="65"/>
+      <c r="S5" s="78"/>
     </row>
     <row r="6" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
@@ -3132,7 +3159,7 @@
       <c r="P6" s="32"/>
       <c r="Q6" s="32"/>
       <c r="R6" s="32"/>
-      <c r="S6" s="66" t="s">
+      <c r="S6" s="79" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3160,7 +3187,7 @@
       <c r="P7" s="38"/>
       <c r="Q7" s="38"/>
       <c r="R7" s="38"/>
-      <c r="S7" s="65"/>
+      <c r="S7" s="78"/>
     </row>
     <row r="8" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -3193,7 +3220,7 @@
       <c r="P8" s="32"/>
       <c r="Q8" s="32"/>
       <c r="R8" s="32"/>
-      <c r="S8" s="66" t="s">
+      <c r="S8" s="79" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3223,7 +3250,7 @@
       <c r="P9" s="38"/>
       <c r="Q9" s="38"/>
       <c r="R9" s="38"/>
-      <c r="S9" s="73"/>
+      <c r="S9" s="85"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
@@ -3231,7 +3258,7 @@
       </c>
       <c r="B10" s="27">
         <f>SUM(D10:R10)</f>
-        <v>0</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="C10" s="28" t="str">
         <f>IF(OR(SUM(D10:O10)=0,$A11=""),"",SUM(D10:O10))</f>
@@ -3243,7 +3270,9 @@
       <c r="G10" s="32"/>
       <c r="H10" s="32"/>
       <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
+      <c r="J10" s="29">
+        <v>0.29166666666666669</v>
+      </c>
       <c r="K10" s="32"/>
       <c r="L10" s="32"/>
       <c r="M10" s="32"/>
@@ -3252,14 +3281,14 @@
       <c r="P10" s="32"/>
       <c r="Q10" s="32"/>
       <c r="R10" s="32"/>
-      <c r="S10" s="66"/>
+      <c r="S10" s="79"/>
     </row>
     <row r="11" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="40"/>
       <c r="B11" s="35"/>
       <c r="C11" s="28">
         <f>SUM(D11:S11)</f>
-        <v>0</v>
+        <v>0.30555555555555552</v>
       </c>
       <c r="D11" s="38"/>
       <c r="E11" s="38"/>
@@ -3267,7 +3296,9 @@
       <c r="G11" s="38"/>
       <c r="H11" s="38"/>
       <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
+      <c r="J11" s="37">
+        <v>0.30555555555555552</v>
+      </c>
       <c r="K11" s="38"/>
       <c r="L11" s="38"/>
       <c r="M11" s="38"/>
@@ -3276,7 +3307,7 @@
       <c r="P11" s="38"/>
       <c r="Q11" s="38"/>
       <c r="R11" s="38"/>
-      <c r="S11" s="73"/>
+      <c r="S11" s="85"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
@@ -3305,7 +3336,7 @@
       <c r="P12" s="32"/>
       <c r="Q12" s="32"/>
       <c r="R12" s="32"/>
-      <c r="S12" s="66"/>
+      <c r="S12" s="79"/>
     </row>
     <row r="13" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="40"/>
@@ -3329,7 +3360,7 @@
       <c r="P13" s="38"/>
       <c r="Q13" s="38"/>
       <c r="R13" s="38"/>
-      <c r="S13" s="73"/>
+      <c r="S13" s="85"/>
     </row>
     <row r="14" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
@@ -3358,7 +3389,7 @@
       <c r="P14" s="32"/>
       <c r="Q14" s="32"/>
       <c r="R14" s="32"/>
-      <c r="S14" s="66"/>
+      <c r="S14" s="79"/>
     </row>
     <row r="15" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="40"/>
@@ -3382,7 +3413,7 @@
       <c r="P15" s="38"/>
       <c r="Q15" s="38"/>
       <c r="R15" s="38"/>
-      <c r="S15" s="73"/>
+      <c r="S15" s="85"/>
     </row>
     <row r="16" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
@@ -3411,7 +3442,7 @@
       <c r="P16" s="32"/>
       <c r="Q16" s="32"/>
       <c r="R16" s="32"/>
-      <c r="S16" s="66"/>
+      <c r="S16" s="79"/>
     </row>
     <row r="17" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="40"/>
@@ -3435,7 +3466,7 @@
       <c r="P17" s="38"/>
       <c r="Q17" s="38"/>
       <c r="R17" s="38"/>
-      <c r="S17" s="73"/>
+      <c r="S17" s="85"/>
     </row>
     <row r="18" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
@@ -3461,7 +3492,7 @@
       <c r="P18" s="32"/>
       <c r="Q18" s="32"/>
       <c r="R18" s="32"/>
-      <c r="S18" s="66"/>
+      <c r="S18" s="79"/>
     </row>
     <row r="19" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="40"/>
@@ -3488,7 +3519,7 @@
       <c r="P19" s="38"/>
       <c r="Q19" s="38"/>
       <c r="R19" s="38"/>
-      <c r="S19" s="73"/>
+      <c r="S19" s="85"/>
     </row>
     <row r="20" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
@@ -3517,7 +3548,7 @@
       <c r="P20" s="32"/>
       <c r="Q20" s="32"/>
       <c r="R20" s="32"/>
-      <c r="S20" s="66"/>
+      <c r="S20" s="79"/>
     </row>
     <row r="21" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
@@ -3544,19 +3575,19 @@
       <c r="P21" s="38"/>
       <c r="Q21" s="38"/>
       <c r="R21" s="38"/>
-      <c r="S21" s="73"/>
+      <c r="S21" s="85"/>
     </row>
     <row r="22" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="67" t="s">
+      <c r="A22" s="80" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="69">
+      <c r="B22" s="82">
         <f>SUM(B4:B21)</f>
-        <v>4.3125</v>
-      </c>
-      <c r="C22" s="79">
+        <v>4.604166666666667</v>
+      </c>
+      <c r="C22" s="65">
         <f>SUM(C5:C21)</f>
-        <v>0.76041666666666674</v>
+        <v>1.0659722222222223</v>
       </c>
       <c r="D22" s="42">
         <f t="shared" ref="D22:R22" si="1">SUM(D4,D6,D8,D10,D12,D14,D16,D18,D20)</f>
@@ -3584,7 +3615,7 @@
       </c>
       <c r="J22" s="43">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="K22" s="43">
         <f t="shared" si="1"/>
@@ -3621,9 +3652,9 @@
       <c r="S22" s="52"/>
     </row>
     <row r="23" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="68"/>
-      <c r="B23" s="70"/>
-      <c r="C23" s="70"/>
+      <c r="A23" s="81"/>
+      <c r="B23" s="66"/>
+      <c r="C23" s="66"/>
       <c r="D23" s="44">
         <f t="shared" ref="D23:R23" si="2">SUM(D5,D7,D9,D11,D13,D15,D17,D19,D21)</f>
         <v>0.125</v>
@@ -3650,7 +3681,7 @@
       </c>
       <c r="J23" s="45">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.30555555555555552</v>
       </c>
       <c r="K23" s="45">
         <f t="shared" si="2"/>
@@ -3744,13 +3775,13 @@
       <c r="S26" s="46"/>
     </row>
     <row r="27" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="80" t="s">
+      <c r="B27" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="81"/>
-      <c r="D27" s="81"/>
-      <c r="E27" s="81"/>
-      <c r="F27" s="82"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="69"/>
       <c r="G27" s="46"/>
       <c r="H27" s="46"/>
       <c r="I27" s="46"/>
@@ -3769,58 +3800,58 @@
       <c r="B28" s="47">
         <v>43513</v>
       </c>
-      <c r="C28" s="83" t="s">
+      <c r="C28" s="70" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="84"/>
-      <c r="E28" s="84"/>
-      <c r="F28" s="85"/>
+      <c r="D28" s="71"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="72"/>
     </row>
     <row r="29" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="48"/>
-      <c r="C29" s="77" t="s">
+      <c r="C29" s="63" t="s">
         <v>69</v>
       </c>
       <c r="D29" s="59"/>
       <c r="E29" s="59"/>
-      <c r="F29" s="78"/>
+      <c r="F29" s="64"/>
     </row>
     <row r="30" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="48"/>
-      <c r="C30" s="77" t="s">
+      <c r="C30" s="63" t="s">
         <v>70</v>
       </c>
       <c r="D30" s="59"/>
       <c r="E30" s="59"/>
-      <c r="F30" s="78"/>
+      <c r="F30" s="64"/>
     </row>
     <row r="31" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="48"/>
-      <c r="C31" s="77" t="s">
+      <c r="C31" s="63" t="s">
         <v>71</v>
       </c>
       <c r="D31" s="59"/>
       <c r="E31" s="59"/>
-      <c r="F31" s="78"/>
+      <c r="F31" s="64"/>
     </row>
     <row r="32" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="48"/>
-      <c r="C32" s="77" t="s">
+      <c r="C32" s="63" t="s">
         <v>72</v>
       </c>
       <c r="D32" s="59"/>
       <c r="E32" s="59"/>
-      <c r="F32" s="78"/>
+      <c r="F32" s="64"/>
     </row>
     <row r="33" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="49"/>
       <c r="B33" s="50"/>
-      <c r="C33" s="74" t="s">
+      <c r="C33" s="60" t="s">
         <v>73</v>
       </c>
-      <c r="D33" s="75"/>
-      <c r="E33" s="75"/>
-      <c r="F33" s="76"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="62"/>
     </row>
     <row r="34" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4791,14 +4822,6 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C31:F31"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="S4:S5"/>
@@ -4813,6 +4836,14 @@
     <mergeCell ref="S16:S17"/>
     <mergeCell ref="S18:S19"/>
     <mergeCell ref="S20:S21"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -4823,8 +4854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5093,33 +5124,73 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="55"/>
-      <c r="B16" s="51"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="51"/>
-    </row>
-    <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="55"/>
-      <c r="B17" s="51"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="51"/>
-    </row>
-    <row r="18" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="55"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="51"/>
-    </row>
-    <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="55"/>
-      <c r="B19" s="51"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="51"/>
+    <row r="16" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A16" s="55">
+        <v>43554</v>
+      </c>
+      <c r="B16" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="51" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" s="55">
+        <v>43556</v>
+      </c>
+      <c r="B17" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" s="51" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A18" s="55">
+        <v>43557</v>
+      </c>
+      <c r="B18" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="51" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="51" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A19" s="55">
+        <v>43558</v>
+      </c>
+      <c r="B19" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" s="56" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="51" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="55"/>

</xml_diff>

<commit_message>
actualizada plantilla de planificacion
</commit_message>
<xml_diff>
--- a/Plantilla_Planificacion/Plantilla_Planificacion_Proyecto.xlsx
+++ b/Plantilla_Planificacion/Plantilla_Planificacion_Proyecto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Industria 4.0\Desktop\Clase\uni1819\Segundo Semestre\Programacion II\Programas2\Plantilla_Planificacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC417569-A880-4861-95F1-759B1B896254}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81C2D27-884F-4F37-A22C-C4E59E6173E0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tareas" sheetId="1" r:id="rId1"/>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="132">
   <si>
     <t>Planificación del proyecto</t>
   </si>
@@ -495,6 +495,33 @@
   </si>
   <si>
     <t>Al tratar de solucionar el que el mismo InternalFrame no se pudiese abrir dos veces hemos encontrado una serie de problemas.</t>
+  </si>
+  <si>
+    <t>Fondo de pantalla</t>
+  </si>
+  <si>
+    <t>No encontrabamos como poner fotos de fondo de pantalla</t>
+  </si>
+  <si>
+    <t>Jtables</t>
+  </si>
+  <si>
+    <t>Problema para entender el funcionamiento de los Jtables e implementarlos en el proyecto</t>
+  </si>
+  <si>
+    <t>Problemas para actualizar los datos en los Jtables</t>
+  </si>
+  <si>
+    <t>Errores con el metodo de ordenamiento</t>
+  </si>
+  <si>
+    <t>Inconformidades con el diseño de las pantallas</t>
+  </si>
+  <si>
+    <t>Mayor desarrollo del esperado para la cantidad de pantallas</t>
+  </si>
+  <si>
+    <t>Prueba de aplicación y correcciones varias</t>
   </si>
 </sst>
 </file>
@@ -1211,7 +1238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1365,6 +1392,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="2" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1387,7 +1437,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1395,28 +1444,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="2" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="46" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1700,7 +1739,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1855,8 +1894,12 @@
       <c r="C12" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="19"/>
+      <c r="D12" s="21">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E12" s="23">
+        <v>6.25E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1876,8 +1919,12 @@
       <c r="C14" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="19"/>
+      <c r="D14" s="21">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E14" s="23">
+        <v>0.91666666666666663</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1897,8 +1944,12 @@
       <c r="C16" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="19"/>
+      <c r="D16" s="21">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E16" s="91">
+        <v>1.25</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -1918,8 +1969,12 @@
       <c r="C18" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="19"/>
+      <c r="D18" s="21">
+        <v>0.625</v>
+      </c>
+      <c r="E18" s="23">
+        <v>0.625</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -1939,8 +1994,8 @@
       <c r="C20" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="19"/>
+      <c r="D20" s="89"/>
+      <c r="E20" s="90"/>
     </row>
     <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="11"/>
@@ -3027,7 +3082,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3035,8 +3090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20:S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3054,10 +3109,10 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="76" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="16" t="s">
@@ -3080,13 +3135,13 @@
       <c r="P2" s="20"/>
       <c r="Q2" s="20"/>
       <c r="R2" s="22"/>
-      <c r="S2" s="65" t="s">
+      <c r="S2" s="78" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="75"/>
-      <c r="B3" s="64"/>
+      <c r="A3" s="87"/>
+      <c r="B3" s="77"/>
       <c r="C3" s="24" t="s">
         <v>42</v>
       </c>
@@ -3149,7 +3204,7 @@
         <f t="shared" si="0"/>
         <v>43605</v>
       </c>
-      <c r="S3" s="66"/>
+      <c r="S3" s="79"/>
     </row>
     <row r="4" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
@@ -3179,7 +3234,7 @@
       <c r="P4" s="32"/>
       <c r="Q4" s="32"/>
       <c r="R4" s="32"/>
-      <c r="S4" s="67" t="s">
+      <c r="S4" s="80" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3206,7 +3261,7 @@
       <c r="P5" s="38"/>
       <c r="Q5" s="38"/>
       <c r="R5" s="38"/>
-      <c r="S5" s="68"/>
+      <c r="S5" s="81"/>
     </row>
     <row r="6" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
@@ -3237,7 +3292,7 @@
       <c r="P6" s="32"/>
       <c r="Q6" s="32"/>
       <c r="R6" s="32"/>
-      <c r="S6" s="69" t="s">
+      <c r="S6" s="82" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3265,7 +3320,7 @@
       <c r="P7" s="38"/>
       <c r="Q7" s="38"/>
       <c r="R7" s="38"/>
-      <c r="S7" s="68"/>
+      <c r="S7" s="81"/>
     </row>
     <row r="8" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
@@ -3298,7 +3353,7 @@
       <c r="P8" s="32"/>
       <c r="Q8" s="32"/>
       <c r="R8" s="32"/>
-      <c r="S8" s="69" t="s">
+      <c r="S8" s="82" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3328,7 +3383,7 @@
       <c r="P9" s="38"/>
       <c r="Q9" s="38"/>
       <c r="R9" s="38"/>
-      <c r="S9" s="76"/>
+      <c r="S9" s="88"/>
     </row>
     <row r="10" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
@@ -3363,7 +3418,7 @@
       <c r="P10" s="32"/>
       <c r="Q10" s="32"/>
       <c r="R10" s="32"/>
-      <c r="S10" s="69" t="s">
+      <c r="S10" s="82" t="s">
         <v>117</v>
       </c>
     </row>
@@ -3395,7 +3450,7 @@
       <c r="P11" s="38"/>
       <c r="Q11" s="38"/>
       <c r="R11" s="38"/>
-      <c r="S11" s="76"/>
+      <c r="S11" s="88"/>
     </row>
     <row r="12" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26" t="s">
@@ -3403,7 +3458,7 @@
       </c>
       <c r="B12" s="27">
         <f>SUM(D12:R12)</f>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="C12" s="28" t="str">
         <f>IF(OR(SUM(D12:O12)=0,$A13=""),"",SUM(D12:O12))</f>
@@ -3417,21 +3472,25 @@
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
       <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="32"/>
+      <c r="L12" s="29">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="M12" s="29"/>
       <c r="N12" s="32"/>
       <c r="O12" s="32"/>
       <c r="P12" s="32"/>
       <c r="Q12" s="32"/>
       <c r="R12" s="32"/>
-      <c r="S12" s="69"/>
+      <c r="S12" s="92" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="13" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="40"/>
       <c r="B13" s="35"/>
       <c r="C13" s="28">
         <f>SUM(D13:S13)</f>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="D13" s="38"/>
       <c r="E13" s="38"/>
@@ -3441,14 +3500,16 @@
       <c r="I13" s="38"/>
       <c r="J13" s="38"/>
       <c r="K13" s="38"/>
-      <c r="L13" s="38"/>
-      <c r="M13" s="38"/>
+      <c r="L13" s="37">
+        <v>6.25E-2</v>
+      </c>
+      <c r="M13" s="37"/>
       <c r="N13" s="38"/>
       <c r="O13" s="38"/>
       <c r="P13" s="38"/>
       <c r="Q13" s="38"/>
       <c r="R13" s="38"/>
-      <c r="S13" s="76"/>
+      <c r="S13" s="88"/>
     </row>
     <row r="14" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
@@ -3456,7 +3517,7 @@
       </c>
       <c r="B14" s="27">
         <f>SUM(D14:R14)</f>
-        <v>0</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="C14" s="28" t="str">
         <f>IF(OR(SUM(D14:O14)=0,$A15=""),"",SUM(D14:O14))</f>
@@ -3470,21 +3531,29 @@
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
       <c r="K14" s="32"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="32"/>
+      <c r="L14" s="29">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="M14" s="29">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="N14" s="29">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="O14" s="32"/>
       <c r="P14" s="32"/>
       <c r="Q14" s="32"/>
       <c r="R14" s="32"/>
-      <c r="S14" s="69"/>
+      <c r="S14" s="92" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="15" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="40"/>
       <c r="B15" s="35"/>
       <c r="C15" s="28">
         <f>SUM(D15:S15)</f>
-        <v>0</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="D15" s="38"/>
       <c r="E15" s="38"/>
@@ -3494,14 +3563,20 @@
       <c r="I15" s="38"/>
       <c r="J15" s="38"/>
       <c r="K15" s="38"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
-      <c r="N15" s="38"/>
+      <c r="L15" s="37">
+        <v>0.22916666666666666</v>
+      </c>
+      <c r="M15" s="37">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="N15" s="37">
+        <v>0.22916666666666666</v>
+      </c>
       <c r="O15" s="38"/>
       <c r="P15" s="38"/>
       <c r="Q15" s="38"/>
       <c r="R15" s="38"/>
-      <c r="S15" s="76"/>
+      <c r="S15" s="88"/>
     </row>
     <row r="16" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
@@ -3509,7 +3584,7 @@
       </c>
       <c r="B16" s="27">
         <f>SUM(D16:R16)</f>
-        <v>0</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="C16" s="28" t="str">
         <f>IF(OR(SUM(D16:O16)=0,$A17=""),"",SUM(D16:O16))</f>
@@ -3524,20 +3599,28 @@
       <c r="J16" s="32"/>
       <c r="K16" s="32"/>
       <c r="L16" s="32"/>
-      <c r="M16" s="32"/>
-      <c r="N16" s="32"/>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="O16" s="29">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="P16" s="29">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="Q16" s="32"/>
       <c r="R16" s="32"/>
-      <c r="S16" s="69"/>
+      <c r="S16" s="92" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="17" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="40"/>
       <c r="B17" s="35"/>
       <c r="C17" s="28">
         <f>SUM(D17:S17)</f>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="D17" s="38"/>
       <c r="E17" s="38"/>
@@ -3548,13 +3631,19 @@
       <c r="J17" s="38"/>
       <c r="K17" s="38"/>
       <c r="L17" s="38"/>
-      <c r="M17" s="38"/>
-      <c r="N17" s="38"/>
-      <c r="O17" s="38"/>
-      <c r="P17" s="38"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="37">
+        <v>0.5</v>
+      </c>
+      <c r="O17" s="37">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="P17" s="37">
+        <v>0.33333333333333331</v>
+      </c>
       <c r="Q17" s="38"/>
       <c r="R17" s="38"/>
-      <c r="S17" s="76"/>
+      <c r="S17" s="88"/>
     </row>
     <row r="18" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
@@ -3562,7 +3651,7 @@
       </c>
       <c r="B18" s="27">
         <f>SUM(D18:R18)</f>
-        <v>0</v>
+        <v>0.625</v>
       </c>
       <c r="C18" s="28"/>
       <c r="D18" s="32"/>
@@ -3575,12 +3664,18 @@
       <c r="K18" s="32"/>
       <c r="L18" s="32"/>
       <c r="M18" s="32"/>
-      <c r="N18" s="32"/>
+      <c r="N18" s="29"/>
       <c r="O18" s="32"/>
       <c r="P18" s="32"/>
-      <c r="Q18" s="32"/>
-      <c r="R18" s="32"/>
-      <c r="S18" s="69"/>
+      <c r="Q18" s="29">
+        <v>0.25</v>
+      </c>
+      <c r="R18" s="29">
+        <v>0.375</v>
+      </c>
+      <c r="S18" s="92" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="19" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="40"/>
@@ -3590,7 +3685,7 @@
       </c>
       <c r="C19" s="28">
         <f>SUM(D19:S19)</f>
-        <v>0</v>
+        <v>0.625</v>
       </c>
       <c r="D19" s="38"/>
       <c r="E19" s="38"/>
@@ -3602,12 +3697,16 @@
       <c r="K19" s="38"/>
       <c r="L19" s="38"/>
       <c r="M19" s="38"/>
-      <c r="N19" s="38"/>
+      <c r="N19" s="37"/>
       <c r="O19" s="38"/>
       <c r="P19" s="38"/>
-      <c r="Q19" s="38"/>
-      <c r="R19" s="38"/>
-      <c r="S19" s="76"/>
+      <c r="Q19" s="37">
+        <v>0.25</v>
+      </c>
+      <c r="R19" s="37">
+        <v>0.375</v>
+      </c>
+      <c r="S19" s="88"/>
     </row>
     <row r="20" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="26" t="s">
@@ -3636,7 +3735,7 @@
       <c r="P20" s="32"/>
       <c r="Q20" s="32"/>
       <c r="R20" s="32"/>
-      <c r="S20" s="69"/>
+      <c r="S20" s="82"/>
     </row>
     <row r="21" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
@@ -3663,19 +3762,19 @@
       <c r="P21" s="38"/>
       <c r="Q21" s="38"/>
       <c r="R21" s="38"/>
-      <c r="S21" s="76"/>
+      <c r="S21" s="88"/>
     </row>
     <row r="22" spans="1:19" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="70" t="s">
+      <c r="A22" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="72">
+      <c r="B22" s="85">
         <f>SUM(B4:B21)</f>
-        <v>4.875</v>
-      </c>
-      <c r="C22" s="82">
+        <v>7.208333333333333</v>
+      </c>
+      <c r="C22" s="68">
         <f>SUM(C5:C21)</f>
-        <v>1.5694444444444446</v>
+        <v>4.4236111111111107</v>
       </c>
       <c r="D22" s="42">
         <f t="shared" ref="D22:R22" si="1">SUM(D4,D6,D8,D10,D12,D14,D16,D18,D20)</f>
@@ -3711,38 +3810,38 @@
       </c>
       <c r="L22" s="43">
         <f t="shared" si="1"/>
-        <v>0.14583333333333334</v>
+        <v>0.39583333333333337</v>
       </c>
       <c r="M22" s="43">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="N22" s="43">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.625</v>
       </c>
       <c r="O22" s="43">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="P22" s="43">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="Q22" s="43">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R22" s="43">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.375</v>
       </c>
       <c r="S22" s="52"/>
     </row>
     <row r="23" spans="1:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="71"/>
-      <c r="B23" s="73"/>
-      <c r="C23" s="73"/>
+      <c r="A23" s="84"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="69"/>
       <c r="D23" s="44">
         <f t="shared" ref="D23:R23" si="2">SUM(D5,D7,D9,D11,D13,D15,D17,D19,D21)</f>
         <v>0.125</v>
@@ -3777,31 +3876,31 @@
       </c>
       <c r="L23" s="45">
         <f t="shared" si="2"/>
-        <v>0.16666666666666666</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="M23" s="45">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="N23" s="45">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.72916666666666663</v>
       </c>
       <c r="O23" s="45">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="P23" s="45">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="Q23" s="45">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R23" s="45">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.375</v>
       </c>
       <c r="S23" s="46"/>
     </row>
@@ -3863,13 +3962,13 @@
       <c r="S26" s="46"/>
     </row>
     <row r="27" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="83" t="s">
+      <c r="B27" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="C27" s="84"/>
-      <c r="D27" s="84"/>
-      <c r="E27" s="84"/>
-      <c r="F27" s="85"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="72"/>
       <c r="G27" s="46"/>
       <c r="H27" s="46"/>
       <c r="I27" s="46"/>
@@ -3888,58 +3987,58 @@
       <c r="B28" s="47">
         <v>43513</v>
       </c>
-      <c r="C28" s="86" t="s">
+      <c r="C28" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="87"/>
-      <c r="E28" s="87"/>
-      <c r="F28" s="88"/>
+      <c r="D28" s="74"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="75"/>
     </row>
     <row r="29" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="48"/>
-      <c r="C29" s="80" t="s">
+      <c r="C29" s="66" t="s">
         <v>69</v>
       </c>
       <c r="D29" s="62"/>
       <c r="E29" s="62"/>
-      <c r="F29" s="81"/>
+      <c r="F29" s="67"/>
     </row>
     <row r="30" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="48"/>
-      <c r="C30" s="80" t="s">
+      <c r="C30" s="66" t="s">
         <v>70</v>
       </c>
       <c r="D30" s="62"/>
       <c r="E30" s="62"/>
-      <c r="F30" s="81"/>
+      <c r="F30" s="67"/>
     </row>
     <row r="31" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="48"/>
-      <c r="C31" s="80" t="s">
+      <c r="C31" s="66" t="s">
         <v>71</v>
       </c>
       <c r="D31" s="62"/>
       <c r="E31" s="62"/>
-      <c r="F31" s="81"/>
+      <c r="F31" s="67"/>
     </row>
     <row r="32" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="48"/>
-      <c r="C32" s="80" t="s">
+      <c r="C32" s="66" t="s">
         <v>72</v>
       </c>
       <c r="D32" s="62"/>
       <c r="E32" s="62"/>
-      <c r="F32" s="81"/>
+      <c r="F32" s="67"/>
     </row>
     <row r="33" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="49"/>
       <c r="B33" s="50"/>
-      <c r="C33" s="77" t="s">
+      <c r="C33" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="D33" s="78"/>
-      <c r="E33" s="78"/>
-      <c r="F33" s="79"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="65"/>
     </row>
     <row r="34" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4910,14 +5009,6 @@
     <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C31:F31"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="S4:S5"/>
@@ -4932,6 +5023,14 @@
     <mergeCell ref="S16:S17"/>
     <mergeCell ref="S18:S19"/>
     <mergeCell ref="S20:S21"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -4942,8 +5041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5331,26 +5430,56 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="55"/>
-      <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="51"/>
-    </row>
-    <row r="24" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="55"/>
-      <c r="B24" s="51"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="51"/>
-    </row>
-    <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="55"/>
-      <c r="B25" s="51"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="51"/>
+    <row r="23" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="55">
+        <v>43592</v>
+      </c>
+      <c r="B23" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="51" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" s="56" t="s">
+        <v>113</v>
+      </c>
+      <c r="E23" s="51" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="55">
+        <v>43595</v>
+      </c>
+      <c r="B24" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="D24" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" s="51" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="55">
+        <v>43600</v>
+      </c>
+      <c r="B25" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="D25" s="56" t="s">
+        <v>113</v>
+      </c>
+      <c r="E25" s="51" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>

</xml_diff>